<commit_message>
put aeay the old code
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="41940" yWindow="0" windowWidth="25600" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="68800" windowHeight="28320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Year of Examination" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="46">
   <si>
     <t>Type of Attribute</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve"> &gt; 20</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -221,8 +224,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -316,7 +333,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="99">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -359,6 +376,13 @@
     <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -401,6 +425,13 @@
     <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -732,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -791,9 +822,6 @@
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>1952</v>
@@ -1298,7 +1326,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1358,7 +1386,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
@@ -1740,10 +1768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1755,7 +1783,7 @@
     <col min="5" max="5" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -1770,7 +1798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1783,8 +1811,17 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2">
+        <v>0.15</v>
+      </c>
+      <c r="F2">
+        <v>0.15</v>
+      </c>
+      <c r="G2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1797,13 +1834,22 @@
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3">
+        <v>0.15</v>
+      </c>
+      <c r="F3">
+        <v>0.15</v>
+      </c>
+      <c r="G3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1811,8 +1857,17 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4">
+        <v>0.3</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1825,8 +1880,17 @@
       <c r="D5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1836,8 +1900,17 @@
       <c r="D6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6">
+        <v>0.3</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1847,8 +1920,17 @@
       <c r="D7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7">
+        <v>0.6</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1975,7 +2057,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2035,7 +2117,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -2207,7 +2289,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2253,7 +2335,7 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>40</v>
@@ -2265,9 +2347,6 @@
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>41</v>

</xml_diff>